<commit_message>
Phase 2. Added memory paging
</commit_message>
<xml_diff>
--- a/Process Stats.xlsx
+++ b/Process Stats.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26940" yWindow="440" windowWidth="41860" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="34400" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Process Timing" sheetId="1" r:id="rId1"/>
     <sheet name="Memory Sizes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -772,11 +772,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1352983392"/>
-        <c:axId val="1367983824"/>
+        <c:axId val="-694099968"/>
+        <c:axId val="-695115600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1352983392"/>
+        <c:axId val="-694099968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1367983824"/>
+        <c:crossAx val="-695115600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -827,7 +827,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1367983824"/>
+        <c:axId val="-695115600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -877,7 +877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1352983392"/>
+        <c:crossAx val="-694099968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -889,6 +889,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1459,11 +1491,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1282673568"/>
-        <c:axId val="1372285984"/>
+        <c:axId val="-694076416"/>
+        <c:axId val="-694073936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1282673568"/>
+        <c:axId val="-694076416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1506,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1372285984"/>
+        <c:crossAx val="-694073936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1514,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1372285984"/>
+        <c:axId val="-694073936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,7 +1596,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1282673568"/>
+        <c:crossAx val="-694076416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1576,6 +1608,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2146,11 +2210,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1374650640"/>
-        <c:axId val="1419008768"/>
+        <c:axId val="-695085232"/>
+        <c:axId val="-695082480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1374650640"/>
+        <c:axId val="-695085232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1419008768"/>
+        <c:crossAx val="-695082480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2201,7 +2265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1419008768"/>
+        <c:axId val="-695082480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1374650640"/>
+        <c:crossAx val="-695085232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2263,6 +2327,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2537,11 +2633,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1451437776"/>
-        <c:axId val="1374511472"/>
+        <c:axId val="-695069104"/>
+        <c:axId val="-695066352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1451437776"/>
+        <c:axId val="-695069104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2584,7 +2680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1374511472"/>
+        <c:crossAx val="-695066352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2592,7 +2688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1374511472"/>
+        <c:axId val="-695066352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2642,7 +2738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1451437776"/>
+        <c:crossAx val="-695069104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2654,6 +2750,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5258,8 +5386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5898,7 +6026,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33">
-        <f t="shared" ref="A33:D33" si="0">AVERAGE(B3:B32)</f>
+        <f t="shared" ref="B33:D33" si="0">AVERAGE(B3:B32)</f>
         <v>14.814933426666668</v>
       </c>
       <c r="C33">
@@ -7223,7 +7351,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>